<commit_message>
Temp resolve confilct (#1029)
update from upstream
</commit_message>
<xml_diff>
--- a/Data/Combat Extended/Combat Extended Armors - 2798914758/2798914758.xlsx
+++ b/Data/Combat Extended/Combat Extended Armors - 2798914758/2798914758.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.7.11\CE Translation\3079466972\Data\Combat Extended\Combat Extended Armors - 2798914758\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Combat Extended\Combat Extended Armors - 2798914758\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA4F581-83F0-41AB-AC23-E50179A16916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4CD963-9137-41C4-9CB2-1E0BA2A3EC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240415" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240603" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -49,18 +49,12 @@
     <t>CE_Armor_LargeBackpack.label</t>
   </si>
   <si>
-    <t>대형 백팩</t>
-  </si>
-  <si>
     <t>ThingDef+CE_Armor_LargeBackpack.description</t>
   </si>
   <si>
     <t>CE_Armor_LargeBackpack.description</t>
   </si>
   <si>
-    <t>등산용 대형 백팩입니다. 산업계 군대의 보병에게 지급되는 종류의 것과 기능상으로 동일합니다.</t>
-  </si>
-  <si>
     <t>ThingDef+CE_Armor_Gambeson.label</t>
   </si>
   <si>
@@ -281,6 +275,12 @@
   </si>
   <si>
     <t>A pair of reinforced goggles capable of stopping shrapnel.</t>
+  </si>
+  <si>
+    <t>등산용 대형 배낭입니다. 산업계 군대의 보병에게 지급되는 종류의 것과 기능상으로 동일합니다.</t>
+  </si>
+  <si>
+    <t>대형 배낭</t>
   </si>
 </sst>
 </file>
@@ -334,7 +334,15 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -635,7 +643,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -680,337 +688,342 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F2:F3">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>(E2=F2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>